<commit_message>
Split the coding scheme into 6 separate surveys to be able to create a formr run (where one article can contain several studies, hypotheses, results). Many formatting tweaks and new variables to cover all potential cases.
IMPORTANT: AssessingRRsPRs_codingscheme_codebook.xlsx is not up to date any more
</commit_message>
<xml_diff>
--- a/AssessingRRsPRs_codingscheme_codebook.xlsx
+++ b/AssessingRRsPRs_codingscheme_codebook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="477">
   <si>
     <t>Category</t>
   </si>
@@ -419,9 +419,6 @@
   </si>
   <si>
     <t>Is this hypothesis part of a replication attempt?</t>
-  </si>
-  <si>
-    <t>HYP_REPLICATION_TYPE_TAX</t>
   </si>
   <si>
     <t>HYP_REPLICATION == 1</t>
@@ -1542,6 +1539,9 @@
   </si>
   <si>
     <t>RESULT_EFF_TYPE == 5</t>
+  </si>
+  <si>
+    <t>HYP_REPLICATION_TYPE_NOTE</t>
   </si>
 </sst>
 </file>
@@ -2442,10 +2442,10 @@
   <dimension ref="A1:V91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D82" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3082,17 +3082,20 @@
       </c>
     </row>
     <row r="21" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
       <c r="C21" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="H21" t="s">
         <v>127</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="K21" t="s">
         <v>129</v>
-      </c>
-      <c r="K21" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="150" x14ac:dyDescent="0.25">
@@ -3103,22 +3106,22 @@
         <v>122</v>
       </c>
       <c r="C22" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" t="s">
         <v>131</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="H22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="H22" t="s">
-        <v>128</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="J22" t="s">
         <v>39</v>
@@ -3127,19 +3130,19 @@
         <v>40</v>
       </c>
       <c r="M22" t="s">
+        <v>135</v>
+      </c>
+      <c r="N22" t="s">
         <v>136</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>137</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>138</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>139</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="60" x14ac:dyDescent="0.25">
@@ -3150,13 +3153,13 @@
         <v>122</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" t="s">
         <v>141</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="F23" t="s">
         <v>25</v>
@@ -3165,10 +3168,10 @@
         <v>52</v>
       </c>
       <c r="H23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K23" t="s">
         <v>27</v>
@@ -3182,10 +3185,10 @@
         <v>122</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" t="s">
         <v>145</v>
-      </c>
-      <c r="D24" t="s">
-        <v>146</v>
       </c>
       <c r="F24" t="s">
         <v>25</v>
@@ -3194,662 +3197,668 @@
         <v>52</v>
       </c>
       <c r="H24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D25" t="s">
-        <v>150</v>
+        <v>153</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="F25" t="s">
-        <v>51</v>
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
+        <v>155</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="K25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" t="s">
         <v>151</v>
       </c>
-      <c r="B26" t="s">
-        <v>152</v>
-      </c>
       <c r="C26" s="9" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
       </c>
-      <c r="H26" t="s">
-        <v>156</v>
-      </c>
       <c r="I26" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="K26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
         <v>151</v>
       </c>
-      <c r="B27" t="s">
-        <v>152</v>
-      </c>
       <c r="C27" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D27" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F27" t="s">
         <v>25</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="K27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D28" t="s">
-        <v>162</v>
-      </c>
-      <c r="F28" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J28" t="s">
+        <v>434</v>
+      </c>
+      <c r="K28" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" t="s">
+        <v>174</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="G29" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" t="s">
+        <v>444</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="K29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>151</v>
-      </c>
-      <c r="B29" t="s">
-        <v>164</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D29" t="s">
-        <v>166</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J29" t="s">
-        <v>435</v>
-      </c>
-      <c r="K29" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>151</v>
-      </c>
-      <c r="B30" t="s">
-        <v>164</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D30" t="s">
-        <v>175</v>
-      </c>
-      <c r="E30" s="1" t="s">
+    <row r="30" spans="1:17" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="H30" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" t="s">
         <v>176</v>
       </c>
-      <c r="F30" t="s">
+      <c r="C31" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D31" t="s">
+        <v>178</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" t="s">
+        <v>102</v>
+      </c>
+      <c r="H31" t="s">
+        <v>445</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K31" t="s">
+        <v>104</v>
+      </c>
+      <c r="M31" t="s">
+        <v>41</v>
+      </c>
+      <c r="N31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D32" t="s">
+        <v>182</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F32" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32" t="s">
+        <v>184</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K32" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" t="s">
+        <v>206</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D33" t="s">
+        <v>208</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H33" t="s">
+        <v>445</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J33" t="s">
+        <v>39</v>
+      </c>
+      <c r="K33" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" t="s">
+        <v>211</v>
+      </c>
+      <c r="N33" t="s">
+        <v>212</v>
+      </c>
+      <c r="O33" t="s">
+        <v>213</v>
+      </c>
+      <c r="P33" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>215</v>
+      </c>
+      <c r="R33" t="s">
+        <v>92</v>
+      </c>
+      <c r="S33" t="s">
+        <v>216</v>
+      </c>
+      <c r="T33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D34" t="s">
+        <v>219</v>
+      </c>
+      <c r="F34" t="s">
         <v>25</v>
       </c>
-      <c r="G30" t="s">
-        <v>52</v>
-      </c>
-      <c r="H30" t="s">
-        <v>445</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="H34" t="s">
+        <v>220</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="K34" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>451</v>
-      </c>
-      <c r="E31" s="13"/>
-      <c r="H31" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>453</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>151</v>
-      </c>
-      <c r="B32" t="s">
-        <v>177</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="D32" t="s">
-        <v>179</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F32" t="s">
-        <v>102</v>
-      </c>
-      <c r="H32" t="s">
-        <v>446</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="K32" t="s">
-        <v>104</v>
-      </c>
-      <c r="M32" t="s">
-        <v>41</v>
-      </c>
-      <c r="N32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>151</v>
-      </c>
-      <c r="B33" t="s">
-        <v>177</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="D33" t="s">
-        <v>183</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F33" t="s">
-        <v>51</v>
-      </c>
-      <c r="H33" t="s">
-        <v>185</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="K33" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" ht="120" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>151</v>
-      </c>
-      <c r="B34" t="s">
-        <v>207</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D34" t="s">
-        <v>209</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="H34" t="s">
-        <v>446</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="J34" t="s">
-        <v>39</v>
-      </c>
-      <c r="K34" t="s">
-        <v>40</v>
-      </c>
-      <c r="M34" t="s">
-        <v>212</v>
-      </c>
-      <c r="N34" t="s">
-        <v>213</v>
-      </c>
-      <c r="O34" t="s">
-        <v>214</v>
-      </c>
-      <c r="P34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>216</v>
-      </c>
-      <c r="R34" t="s">
-        <v>92</v>
-      </c>
-      <c r="S34" t="s">
-        <v>217</v>
-      </c>
-      <c r="T34" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D35" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F35" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="H35" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="K35" t="s">
-        <v>27</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D36" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F36" t="s">
         <v>51</v>
       </c>
       <c r="H36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I36" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K36" t="s">
         <v>226</v>
-      </c>
-      <c r="K36" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B37" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D37" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F37" t="s">
         <v>51</v>
       </c>
       <c r="H37" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="K37" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D38" t="s">
-        <v>232</v>
-      </c>
-      <c r="F38" t="s">
+        <v>236</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H38" t="s">
+        <v>445</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="J38" t="s">
+        <v>39</v>
+      </c>
+      <c r="K38" t="s">
+        <v>40</v>
+      </c>
+      <c r="M38" t="s">
+        <v>240</v>
+      </c>
+      <c r="N38" t="s">
+        <v>241</v>
+      </c>
+      <c r="O38" t="s">
+        <v>242</v>
+      </c>
+      <c r="P38" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>216</v>
+      </c>
+      <c r="R38" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" t="s">
+        <v>234</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D39" t="s">
+        <v>245</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F39" t="s">
         <v>51</v>
       </c>
-      <c r="H38" t="s">
-        <v>233</v>
-      </c>
-      <c r="I38" s="1" t="s">
+      <c r="H39" t="s">
+        <v>247</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" t="s">
         <v>234</v>
       </c>
-      <c r="K38" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>151</v>
-      </c>
-      <c r="B39" t="s">
-        <v>235</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D39" t="s">
-        <v>237</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="H39" t="s">
-        <v>446</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="J39" t="s">
-        <v>39</v>
-      </c>
-      <c r="K39" t="s">
-        <v>40</v>
-      </c>
-      <c r="M39" t="s">
-        <v>241</v>
-      </c>
-      <c r="N39" t="s">
-        <v>242</v>
-      </c>
-      <c r="O39" t="s">
-        <v>243</v>
-      </c>
-      <c r="P39" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>217</v>
-      </c>
-      <c r="R39" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>151</v>
-      </c>
-      <c r="B40" t="s">
-        <v>235</v>
-      </c>
       <c r="C40" s="9" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="D40" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="F40" t="s">
         <v>51</v>
       </c>
       <c r="H40" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="K40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D41" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="F41" t="s">
         <v>51</v>
       </c>
       <c r="H41" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="K41" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="H42" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>453</v>
+      </c>
+      <c r="K42" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>151</v>
-      </c>
-      <c r="B42" t="s">
-        <v>235</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="D42" t="s">
-        <v>256</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F42" t="s">
-        <v>51</v>
-      </c>
-      <c r="H42" t="s">
-        <v>258</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="K42" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>452</v>
-      </c>
-      <c r="E43" s="13"/>
-      <c r="H43" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>454</v>
-      </c>
-      <c r="K43" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>188</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F43" t="s">
+        <v>102</v>
+      </c>
+      <c r="H43" t="s">
+        <v>446</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K43" t="s">
+        <v>104</v>
+      </c>
+      <c r="M43" t="s">
+        <v>41</v>
+      </c>
+      <c r="N43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D44" t="s">
-        <v>189</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F44" t="s">
-        <v>102</v>
+        <v>192</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="H44" t="s">
-        <v>447</v>
+        <v>194</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
+      </c>
+      <c r="J44" t="s">
+        <v>39</v>
       </c>
       <c r="K44" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="M44" t="s">
-        <v>41</v>
+        <v>196</v>
       </c>
       <c r="N44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D45" t="s">
-        <v>193</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F45" t="s">
+        <v>25</v>
       </c>
       <c r="H45" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="J45" t="s">
-        <v>39</v>
+        <v>201</v>
       </c>
       <c r="K45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M45" t="s">
-        <v>197</v>
-      </c>
-      <c r="N45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D46" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F46" t="s">
         <v>25</v>
       </c>
       <c r="H46" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>202</v>
+        <v>97</v>
       </c>
       <c r="K46" t="s">
         <v>27</v>
@@ -3857,28 +3866,28 @@
     </row>
     <row r="47" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>177</v>
+        <v>343</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>203</v>
+        <v>344</v>
       </c>
       <c r="D47" t="s">
-        <v>204</v>
+        <v>345</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>205</v>
+        <v>346</v>
       </c>
       <c r="F47" t="s">
         <v>25</v>
       </c>
       <c r="H47" t="s">
-        <v>206</v>
+        <v>447</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>97</v>
+        <v>347</v>
       </c>
       <c r="K47" t="s">
         <v>27</v>
@@ -3886,275 +3895,278 @@
     </row>
     <row r="48" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="D48" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="F48" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="H48" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="K48" t="s">
-        <v>27</v>
+        <v>104</v>
+      </c>
+      <c r="M48" t="s">
+        <v>41</v>
+      </c>
+      <c r="N48" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B49" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="D49" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F49" t="s">
-        <v>102</v>
+        <v>354</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>355</v>
       </c>
       <c r="H49" t="s">
-        <v>448</v>
+        <v>356</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>352</v>
+        <v>357</v>
+      </c>
+      <c r="J49" t="s">
+        <v>39</v>
       </c>
       <c r="K49" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="M49" t="s">
-        <v>41</v>
+        <v>358</v>
       </c>
       <c r="N49" t="s">
-        <v>42</v>
+        <v>92</v>
+      </c>
+      <c r="O49" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B50" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="D50" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>356</v>
+        <v>361</v>
+      </c>
+      <c r="F50" t="s">
+        <v>25</v>
       </c>
       <c r="H50" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="J50" t="s">
-        <v>39</v>
+        <v>363</v>
       </c>
       <c r="K50" t="s">
-        <v>40</v>
-      </c>
-      <c r="M50" t="s">
-        <v>359</v>
-      </c>
-      <c r="N50" t="s">
-        <v>92</v>
-      </c>
-      <c r="O50" t="s">
-        <v>218</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B51" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="D51" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="F51" t="s">
         <v>25</v>
       </c>
       <c r="H51" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="K51" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B52" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D52" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="F52" t="s">
+        <v>370</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H52" t="s">
+        <v>356</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="K52" t="s">
+        <v>104</v>
+      </c>
+      <c r="M52" t="s">
+        <v>372</v>
+      </c>
+      <c r="N52" t="s">
+        <v>373</v>
+      </c>
+      <c r="O52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" t="s">
+        <v>343</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="D53" t="s">
+        <v>375</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F53" t="s">
         <v>25</v>
       </c>
-      <c r="H52" t="s">
-        <v>357</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="K52" t="s">
+      <c r="H53" t="s">
+        <v>377</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="K53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>151</v>
-      </c>
-      <c r="B53" t="s">
-        <v>344</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="D53" t="s">
-        <v>370</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="H53" t="s">
-        <v>357</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="K53" t="s">
-        <v>104</v>
-      </c>
-      <c r="M53" t="s">
-        <v>373</v>
-      </c>
-      <c r="N53" t="s">
-        <v>374</v>
-      </c>
-      <c r="O53" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="D54" t="s">
-        <v>376</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="F54" t="s">
+        <v>51</v>
+      </c>
+      <c r="H54" t="s">
+        <v>356</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="K54" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55" t="s">
+        <v>343</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="D55" t="s">
+        <v>383</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F55" t="s">
         <v>25</v>
       </c>
-      <c r="H54" t="s">
-        <v>378</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="K54" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>151</v>
-      </c>
-      <c r="B55" t="s">
-        <v>344</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>379</v>
-      </c>
-      <c r="D55" t="s">
-        <v>380</v>
-      </c>
-      <c r="F55" t="s">
-        <v>51</v>
+      <c r="G55" t="s">
+        <v>52</v>
       </c>
       <c r="H55" t="s">
-        <v>357</v>
+        <v>447</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="K55" t="s">
-        <v>382</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B56" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="D56" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="F56" t="s">
         <v>25</v>
@@ -4163,219 +4175,228 @@
         <v>52</v>
       </c>
       <c r="H56" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="K56" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s">
-        <v>344</v>
+        <v>259</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>387</v>
+        <v>260</v>
       </c>
       <c r="D57" t="s">
-        <v>388</v>
+        <v>261</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>389</v>
+        <v>262</v>
       </c>
       <c r="F57" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="G57" t="s">
         <v>52</v>
       </c>
-      <c r="H57" t="s">
-        <v>448</v>
-      </c>
       <c r="I57" s="1" t="s">
-        <v>390</v>
+        <v>263</v>
       </c>
       <c r="K57" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D58" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="F58" t="s">
-        <v>51</v>
-      </c>
-      <c r="G58" t="s">
-        <v>52</v>
+        <v>266</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="K58" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="M58" t="s">
+        <v>269</v>
+      </c>
+      <c r="N58" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="D59" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>268</v>
+        <v>273</v>
+      </c>
+      <c r="F59" t="s">
+        <v>25</v>
+      </c>
+      <c r="H59" t="s">
+        <v>274</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="K59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" t="s">
+        <v>259</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D60" t="s">
+        <v>277</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F60" t="s">
+        <v>102</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="K60" t="s">
         <v>104</v>
       </c>
-      <c r="M59" t="s">
-        <v>270</v>
-      </c>
-      <c r="N59" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>151</v>
-      </c>
-      <c r="B60" t="s">
-        <v>260</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="D60" t="s">
-        <v>273</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F60" t="s">
-        <v>25</v>
-      </c>
-      <c r="H60" t="s">
-        <v>275</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="K60" t="s">
-        <v>27</v>
+      <c r="M60" t="s">
+        <v>41</v>
+      </c>
+      <c r="N60" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B61" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D61" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="F61" t="s">
-        <v>102</v>
+        <v>25</v>
+      </c>
+      <c r="H61" t="s">
+        <v>283</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="K61" t="s">
-        <v>104</v>
-      </c>
-      <c r="M61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>150</v>
+      </c>
+      <c r="B62" t="s">
+        <v>259</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="D62" t="s">
+        <v>286</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F62" t="s">
+        <v>37</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="J62" t="s">
+        <v>39</v>
+      </c>
+      <c r="K62" t="s">
+        <v>40</v>
+      </c>
+      <c r="M62" t="s">
         <v>41</v>
       </c>
-      <c r="N61" t="s">
+      <c r="N62" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>151</v>
-      </c>
-      <c r="B62" t="s">
-        <v>260</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="D62" t="s">
-        <v>282</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F62" t="s">
-        <v>25</v>
-      </c>
-      <c r="H62" t="s">
-        <v>284</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="K62" t="s">
-        <v>60</v>
+      <c r="O62" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B63" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D63" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F63" t="s">
         <v>37</v>
       </c>
+      <c r="H63" t="s">
+        <v>292</v>
+      </c>
       <c r="I63" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="J63" t="s">
         <v>39</v>
@@ -4395,60 +4416,48 @@
     </row>
     <row r="64" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B64" t="s">
-        <v>260</v>
+        <v>293</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D64" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="F64" t="s">
-        <v>37</v>
-      </c>
-      <c r="H64" t="s">
+        <v>51</v>
+      </c>
+      <c r="G64" t="s">
+        <v>52</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="K64" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>150</v>
+      </c>
+      <c r="B65" t="s">
         <v>293</v>
       </c>
-      <c r="I64" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="J64" t="s">
-        <v>39</v>
-      </c>
-      <c r="K64" t="s">
-        <v>40</v>
-      </c>
-      <c r="M64" t="s">
-        <v>41</v>
-      </c>
-      <c r="N64" t="s">
-        <v>42</v>
-      </c>
-      <c r="O64" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>151</v>
-      </c>
-      <c r="B65" t="s">
-        <v>294</v>
-      </c>
       <c r="C65" s="9" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D65" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="F65" t="s">
         <v>51</v>
@@ -4457,7 +4466,7 @@
         <v>52</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="K65" t="s">
         <v>55</v>
@@ -4465,136 +4474,148 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B66" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D66" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="F66" t="s">
-        <v>51</v>
-      </c>
-      <c r="G66" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="I66" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="K66" t="s">
+        <v>104</v>
+      </c>
+      <c r="M66" t="s">
+        <v>41</v>
+      </c>
+      <c r="N66" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>150</v>
+      </c>
+      <c r="B67" t="s">
         <v>302</v>
       </c>
-      <c r="K66" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>151</v>
-      </c>
-      <c r="B67" t="s">
-        <v>303</v>
-      </c>
       <c r="C67" s="9" t="s">
-        <v>304</v>
+        <v>454</v>
       </c>
       <c r="D67" t="s">
-        <v>305</v>
+        <v>455</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="F67" t="s">
-        <v>102</v>
+        <v>456</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="H67" t="s">
+        <v>337</v>
       </c>
       <c r="I67" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="O67" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="P67" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>150</v>
+      </c>
+      <c r="B68" t="s">
+        <v>302</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="K67" t="s">
-        <v>104</v>
-      </c>
-      <c r="M67" t="s">
-        <v>41</v>
-      </c>
-      <c r="N67" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" ht="75" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>151</v>
-      </c>
-      <c r="B68" t="s">
-        <v>303</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>455</v>
-      </c>
       <c r="D68" t="s">
-        <v>456</v>
+        <v>308</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>457</v>
+        <v>309</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>459</v>
+        <v>310</v>
       </c>
       <c r="H68" t="s">
-        <v>338</v>
+        <v>462</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="J68" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J68" t="s">
         <v>39</v>
       </c>
-      <c r="K68" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="M68" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="N68" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="O68" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="P68" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="Q68" t="s">
+      <c r="K68" t="s">
+        <v>40</v>
+      </c>
+      <c r="M68" t="s">
+        <v>312</v>
+      </c>
+      <c r="N68" t="s">
+        <v>313</v>
+      </c>
+      <c r="O68" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B69" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C69" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="D69" t="s">
         <v>308</v>
       </c>
-      <c r="D69" t="s">
-        <v>309</v>
-      </c>
       <c r="E69" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="H69" t="s">
         <v>463</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J69" t="s">
         <v>39</v>
@@ -4603,39 +4624,42 @@
         <v>40</v>
       </c>
       <c r="M69" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="N69" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="O69" t="s">
+        <v>319</v>
+      </c>
+      <c r="P69" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q69" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B70" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="D70" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="H70" t="s">
         <v>464</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J70" t="s">
         <v>39</v>
@@ -4644,42 +4668,45 @@
         <v>40</v>
       </c>
       <c r="M70" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="N70" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="O70" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="P70" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="Q70" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B71" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D71" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="H71" t="s">
         <v>465</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J71" t="s">
         <v>39</v>
@@ -4688,80 +4715,62 @@
         <v>40</v>
       </c>
       <c r="M71" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="N71" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="O71" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="P71" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q71" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B72" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>328</v>
+        <v>470</v>
       </c>
       <c r="D72" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>330</v>
+        <v>334</v>
+      </c>
+      <c r="F72" t="s">
+        <v>25</v>
       </c>
       <c r="H72" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="J72" t="s">
-        <v>39</v>
+        <v>311</v>
       </c>
       <c r="K72" t="s">
-        <v>40</v>
-      </c>
-      <c r="M72" t="s">
-        <v>331</v>
-      </c>
-      <c r="N72" t="s">
-        <v>332</v>
-      </c>
-      <c r="O72" t="s">
-        <v>333</v>
-      </c>
-      <c r="P72" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
     </row>
     <row r="73" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B73" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>471</v>
       </c>
       <c r="D73" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F73" t="s">
         <v>25</v>
@@ -4770,7 +4779,7 @@
         <v>468</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K73" t="s">
         <v>27</v>
@@ -4778,28 +4787,28 @@
     </row>
     <row r="74" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B74" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>472</v>
       </c>
       <c r="D74" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F74" t="s">
         <v>25</v>
       </c>
       <c r="H74" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K74" t="s">
         <v>27</v>
@@ -4807,28 +4816,28 @@
     </row>
     <row r="75" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B75" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F75" t="s">
         <v>25</v>
       </c>
       <c r="H75" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K75" t="s">
         <v>27</v>
@@ -4836,338 +4845,332 @@
     </row>
     <row r="76" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B76" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>475</v>
+        <v>333</v>
       </c>
       <c r="D76" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F76" t="s">
         <v>25</v>
       </c>
       <c r="H76" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K76" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B77" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D77" t="s">
-        <v>309</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F77" t="s">
+        <v>51</v>
+      </c>
+      <c r="H77" t="s">
+        <v>337</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="K77" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>150</v>
+      </c>
+      <c r="B78" t="s">
+        <v>302</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="D78" t="s">
+        <v>339</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F78" t="s">
         <v>25</v>
       </c>
-      <c r="H77" t="s">
-        <v>476</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="K77" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>151</v>
-      </c>
-      <c r="B78" t="s">
-        <v>303</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="D78" t="s">
-        <v>337</v>
-      </c>
-      <c r="F78" t="s">
-        <v>51</v>
+      <c r="G78" t="s">
+        <v>52</v>
       </c>
       <c r="H78" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>467</v>
+        <v>342</v>
       </c>
       <c r="K78" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B79" t="s">
-        <v>303</v>
+        <v>109</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>339</v>
+        <v>390</v>
       </c>
       <c r="D79" t="s">
-        <v>340</v>
+        <v>391</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F79" t="s">
-        <v>25</v>
-      </c>
-      <c r="G79" t="s">
-        <v>52</v>
-      </c>
-      <c r="H79" t="s">
-        <v>342</v>
+        <v>392</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>343</v>
+        <v>393</v>
       </c>
       <c r="K79" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="M79" t="s">
+        <v>117</v>
+      </c>
+      <c r="N79" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B80" t="s">
         <v>109</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D80" t="s">
-        <v>392</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>113</v>
+        <v>395</v>
+      </c>
+      <c r="F80" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" t="s">
+        <v>52</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="K80" t="s">
-        <v>116</v>
-      </c>
-      <c r="M80" t="s">
-        <v>117</v>
-      </c>
-      <c r="N80" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>151</v>
+        <v>397</v>
       </c>
       <c r="B81" t="s">
-        <v>109</v>
+        <v>398</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="D81" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="F81" t="s">
         <v>25</v>
       </c>
-      <c r="G81" t="s">
-        <v>52</v>
-      </c>
       <c r="I81" s="1" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="K81" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="150" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>397</v>
+      </c>
+      <c r="B82" t="s">
         <v>398</v>
       </c>
-      <c r="B82" t="s">
-        <v>399</v>
-      </c>
       <c r="C82" s="9" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D82" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="F82" t="s">
         <v>25</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="K82" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B83" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="D83" t="s">
-        <v>404</v>
-      </c>
-      <c r="F83" t="s">
-        <v>25</v>
+        <v>407</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>408</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>405</v>
+        <v>409</v>
+      </c>
+      <c r="J83" t="s">
+        <v>39</v>
       </c>
       <c r="K83" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="M83" t="s">
+        <v>410</v>
+      </c>
+      <c r="N83" t="s">
+        <v>411</v>
+      </c>
+      <c r="O83" t="s">
+        <v>412</v>
+      </c>
+      <c r="P83" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>91</v>
+      </c>
+      <c r="R83" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B84" t="s">
-        <v>406</v>
+        <v>109</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="D84" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>83</v>
+        <v>415</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>409</v>
+        <v>113</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="J84" t="s">
-        <v>39</v>
+        <v>393</v>
       </c>
       <c r="K84" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="M84" t="s">
-        <v>411</v>
+        <v>117</v>
       </c>
       <c r="N84" t="s">
-        <v>412</v>
-      </c>
-      <c r="O84" t="s">
-        <v>413</v>
-      </c>
-      <c r="P84" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q84" t="s">
-        <v>91</v>
-      </c>
-      <c r="R84" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B85" t="s">
         <v>109</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D85" t="s">
-        <v>415</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>113</v>
+        <v>417</v>
+      </c>
+      <c r="F85" t="s">
+        <v>25</v>
+      </c>
+      <c r="G85" t="s">
+        <v>52</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="K85" t="s">
-        <v>116</v>
-      </c>
-      <c r="M85" t="s">
-        <v>117</v>
-      </c>
-      <c r="N85" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>398</v>
-      </c>
-      <c r="B86" t="s">
-        <v>109</v>
+        <v>418</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D86" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="F86" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="G86" t="s">
         <v>52</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>397</v>
+        <v>421</v>
       </c>
       <c r="K86" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D87" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="F87" t="s">
         <v>51</v>
@@ -5176,7 +5179,7 @@
         <v>52</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="K87" t="s">
         <v>55</v>
@@ -5184,22 +5187,22 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>419</v>
+        <v>22</v>
+      </c>
+      <c r="B88" t="s">
+        <v>147</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>423</v>
+        <v>148</v>
       </c>
       <c r="D88" t="s">
-        <v>424</v>
+        <v>149</v>
       </c>
       <c r="F88" t="s">
         <v>51</v>
       </c>
-      <c r="G88" t="s">
-        <v>52</v>
-      </c>
       <c r="I88" s="1" t="s">
-        <v>425</v>
+        <v>149</v>
       </c>
       <c r="K88" t="s">
         <v>55</v>
@@ -5213,16 +5216,16 @@
         <v>68</v>
       </c>
       <c r="C89" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="D89" t="s">
         <v>426</v>
-      </c>
-      <c r="D89" t="s">
-        <v>427</v>
       </c>
       <c r="F89" t="s">
         <v>51</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K89" t="s">
         <v>55</v>
@@ -5236,19 +5239,19 @@
         <v>109</v>
       </c>
       <c r="C90" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="D90" t="s">
         <v>429</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>431</v>
       </c>
       <c r="F90" t="s">
         <v>37</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J90" t="s">
         <v>39</v>
@@ -5271,10 +5274,10 @@
         <v>22</v>
       </c>
       <c r="C91" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="D91" t="s">
         <v>432</v>
-      </c>
-      <c r="D91" t="s">
-        <v>433</v>
       </c>
       <c r="F91" t="s">
         <v>25</v>
@@ -5283,7 +5286,7 @@
         <v>52</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K91" t="s">
         <v>60</v>
@@ -5318,10 +5321,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>436</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>437</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -5332,46 +5335,46 @@
     </row>
     <row r="2" spans="1:4" ht="174" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>439</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="5"/>
       <c r="C5" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>